<commit_message>
Added TC2 and related amendments
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/data/TestData.xlsx
+++ b/src/main/java/com/qa/data/TestData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zheny\IdeaProjects\AutomationExerciseTesting\src\main\java\com\qa\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA438015-317C-429D-B986-4DF3C2A70F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7063B25-9668-4C79-B81F-36D104D2C697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4524" yWindow="2436" windowWidth="17280" windowHeight="9960" xr2:uid="{2C8DF1BF-95D3-4F94-9E51-20D4FB67B8D7}"/>
+    <workbookView xWindow="4524" yWindow="2436" windowWidth="17280" windowHeight="9960" activeTab="2" xr2:uid="{2C8DF1BF-95D3-4F94-9E51-20D4FB67B8D7}"/>
   </bookViews>
   <sheets>
     <sheet name="RegistrationData" sheetId="1" r:id="rId1"/>
-    <sheet name="LoginData" sheetId="2" r:id="rId2"/>
+    <sheet name="CorrectLoginData" sheetId="2" r:id="rId2"/>
+    <sheet name="IncorrectLoginData" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>email</t>
   </si>
@@ -121,6 +122,24 @@
   </si>
   <si>
     <t>name+O:OQ2A:Q</t>
+  </si>
+  <si>
+    <t>eve1</t>
+  </si>
+  <si>
+    <t>eve1@gmail.com</t>
+  </si>
+  <si>
+    <t>marina@gmail.com</t>
+  </si>
+  <si>
+    <t>123123</t>
+  </si>
+  <si>
+    <t>artem@gmail.com</t>
+  </si>
+  <si>
+    <t>qqq</t>
   </si>
 </sst>
 </file>
@@ -484,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8772A4-31AD-4881-AC31-5675D8A0BBCF}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -603,23 +622,160 @@
         <v>123123123</v>
       </c>
     </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1">
+        <v>123123</v>
+      </c>
+      <c r="E3" s="1">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1984</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="1">
+        <v>123</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>123123123</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{7E5868AF-7D1E-41D7-A09E-D460772F7538}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00A13278-C2AD-489C-9D8A-CCC32FB2793C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B861FE01-7953-40E7-B1FC-26750D1B0BBF}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{2EC5EEEB-57C3-4FF5-AEFB-4D595587B0ED}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{265A039D-5AE5-4736-8516-A5E34713FB56}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA9821D-8B2D-45CA-A5E3-8D6FC200FF76}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20" style="1" customWidth="1"/>
+    <col min="2" max="4" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1">
+        <v>123123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="1">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{08EACCAB-044E-4772-95C3-09EF84524FE3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>